<commit_message>
Updated Formal Requirements Excel Sheet
</commit_message>
<xml_diff>
--- a/03_Formal_Requirements.xlsx
+++ b/03_Formal_Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpoel\Documents\EE_Projects\CHG_USB_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpoel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB08132-AA47-405E-9BB5-8C561012CD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C88AA4E-5457-40D1-A428-E58165180476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26010" windowHeight="20820" xr2:uid="{47DA02D3-0374-495E-8332-452ED06CFF5E}"/>
+    <workbookView xWindow="3900" yWindow="780" windowWidth="26010" windowHeight="20820" xr2:uid="{47DA02D3-0374-495E-8332-452ED06CFF5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t xml:space="preserve">Project Name: CHG_USB_A_CHARGER </t>
   </si>
@@ -116,21 +116,9 @@
     <t>CHG-ME-0003</t>
   </si>
   <si>
-    <t>CHG-ME-0004</t>
-  </si>
-  <si>
     <t>CHG-EE-0005</t>
   </si>
   <si>
-    <t>CHG-EE-0006</t>
-  </si>
-  <si>
-    <t>Device shall include an LED to indicate power is present.</t>
-  </si>
-  <si>
-    <t>Apply input voltage and visually confirm LED.</t>
-  </si>
-  <si>
     <t>Device shall receive input power via a 2.1mm barrel jack.</t>
   </si>
   <si>
@@ -143,19 +131,13 @@
     <t>Measure hole size and spacing in layout.</t>
   </si>
   <si>
-    <t>Inspect PCB layout orientation in Altium Designer.</t>
-  </si>
-  <si>
-    <t>Status: In Progress as of 30 June 2025</t>
-  </si>
-  <si>
     <t>Device shall provide at least 2.2A of output current.</t>
   </si>
   <si>
     <t>PCB shall include a USB-C port accessible from one edge.</t>
   </si>
   <si>
-    <t>USB-C port and LED shall be placed on the same board edge.</t>
+    <t>Status: In Progress as of 4 September 2025</t>
   </si>
 </sst>
 </file>
@@ -179,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -234,17 +216,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -280,8 +251,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1EA83C-838C-4B99-9E0E-0BCF3A5FA728}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,31 +602,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="9"/>
+      <c r="A4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -690,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -729,87 +700,65 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>19</v>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>